<commit_message>
home page and fixtures
</commit_message>
<xml_diff>
--- a/domainapp/example/dom/src/main/java/org/incode/domainapp/example/dom/demo/fixture/todoitems/MoreToDoItems.xlsx
+++ b/domainapp/example/dom/src/main/java/org/incode/domainapp/example/dom/demo/fixture/todoitems/MoreToDoItems.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\isisaddons\isis-module-excel\fixture\src\main\java\org\isisaddons\module\excel\fixture\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\incodehq\incode-platform\domainapp\example\dom\src\main\java\org\incode\domainapp\example\dom\demo\fixture\todoitems\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="19155" windowHeight="10305"/>
   </bookViews>
   <sheets>
-    <sheet name="ExcelModuleDemoToDoItem" sheetId="1" r:id="rId1"/>
+    <sheet name="DemoToDoItem" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -208,6 +208,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -243,6 +260,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,7 +459,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>